<commit_message>
Cambios actualizados de proyecto con excel
</commit_message>
<xml_diff>
--- a/build/resources/test/datadriven/TEST_EXCEL_ID.xlsx
+++ b/build/resources/test/datadriven/TEST_EXCEL_ID.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scastaño\Bancolombia projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scastaño\Bancolombia projects\Exercise_Excel_Forms\src\test\resources\datadriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B9D010B-8406-401C-8DDF-F7164DF1651F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4AC1616D-C2AF-48ED-8C0A-045A9555AB7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,28 +20,73 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>1,Sara,Castano,20,CC,1001227827</t>
-  </si>
-  <si>
-    <t>2,Mario,Rodriguez,19,CC,1001234734</t>
-  </si>
-  <si>
-    <t>3,Marta,Sierra,23,CC,3443378853</t>
-  </si>
-  <si>
-    <t>4,Camilo,Correa,55,CC,3747474299</t>
-  </si>
-  <si>
-    <t>filtro,name,last_name,age,type_document,number_document</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+  <si>
+    <t>filtro</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>current_address</t>
+  </si>
+  <si>
+    <t>permanent_address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alexis Castano </t>
+  </si>
+  <si>
+    <t>Sara Montoya</t>
+  </si>
+  <si>
+    <t>Manuela Restrepo</t>
+  </si>
+  <si>
+    <t>Susana Quiroz</t>
+  </si>
+  <si>
+    <t>AlexisCastano@gmail.com</t>
+  </si>
+  <si>
+    <t>SaraMontoya@gmail.com</t>
+  </si>
+  <si>
+    <t>ManuelaRestrepo@gmail.com</t>
+  </si>
+  <si>
+    <t>SusanaQuiroz@gmail.com</t>
+  </si>
+  <si>
+    <t>cll324 sur 10</t>
+  </si>
+  <si>
+    <t>cll389 sur 11</t>
+  </si>
+  <si>
+    <t>cll382 sur 12</t>
+  </si>
+  <si>
+    <t>cll394 sur 13</t>
+  </si>
+  <si>
+    <t>cll389 sur 12</t>
+  </si>
+  <si>
+    <t>cll382 sur 13</t>
+  </si>
+  <si>
+    <t>cll394 sur 14</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +217,20 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -474,7 +533,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -517,11 +576,13 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -553,6 +614,7 @@
     <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Hipervínculo" xfId="42" builtinId="8"/>
     <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -875,39 +937,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{A29A09F9-5E24-4921-8574-09AB690D07AB}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{E2B3C26E-7E75-4D88-A192-8348E94F9C21}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{0C901AAB-F6CF-44FF-BEFD-0E165D7E1C61}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{3B9FA342-A28B-42E1-B9DF-5FD019176F48}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>